<commit_message>
Correccion de campos decimales y fecha de liquidacion
</commit_message>
<xml_diff>
--- a/db/excel/data.xlsx
+++ b/db/excel/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="817" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-21720" yWindow="-885" windowWidth="21840" windowHeight="13140" tabRatio="817" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS EMPLEADOS" sheetId="1" state="visible" r:id="rId1"/>
@@ -643,10 +643,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3654,8 +3654,8 @@
   </sheetPr>
   <dimension ref="A2:CE14"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -3862,10 +3862,10 @@
     </row>
     <row r="3" ht="25.5" customFormat="1" customHeight="1" s="78">
       <c r="A3" s="94" t="n"/>
-      <c r="B3" s="101" t="n"/>
+      <c r="B3" s="102" t="n"/>
       <c r="C3" s="94" t="n"/>
       <c r="D3" s="94" t="n"/>
-      <c r="E3" s="101" t="n"/>
+      <c r="E3" s="102" t="n"/>
       <c r="F3" s="94" t="n"/>
       <c r="G3" s="94" t="n"/>
       <c r="H3" s="94" t="n"/>
@@ -4000,10 +4000,10 @@
     </row>
     <row r="4" ht="38.25" customFormat="1" customHeight="1" s="80">
       <c r="A4" s="94" t="n"/>
-      <c r="B4" s="101" t="n"/>
+      <c r="B4" s="102" t="n"/>
       <c r="C4" s="94" t="n"/>
       <c r="D4" s="94" t="n"/>
-      <c r="E4" s="101" t="n"/>
+      <c r="E4" s="102" t="n"/>
       <c r="F4" s="94" t="n"/>
       <c r="G4" s="94" t="n"/>
       <c r="H4" s="94" t="n"/>
@@ -4018,10 +4018,10 @@
       <c r="Q4" s="94" t="n"/>
       <c r="R4" s="94" t="n"/>
       <c r="S4" s="94" t="n"/>
-      <c r="T4" s="101" t="n"/>
-      <c r="U4" s="101" t="n"/>
-      <c r="V4" s="101" t="n"/>
-      <c r="W4" s="101" t="n"/>
+      <c r="T4" s="102" t="n"/>
+      <c r="U4" s="102" t="n"/>
+      <c r="V4" s="102" t="n"/>
+      <c r="W4" s="102" t="n"/>
       <c r="X4" s="97" t="n"/>
       <c r="Y4" s="117" t="n"/>
       <c r="Z4" s="9" t="n">
@@ -4083,7 +4083,7 @@
       <c r="AY4" s="4" t="n">
         <v>0.04</v>
       </c>
-      <c r="AZ4" s="102" t="inlineStr">
+      <c r="AZ4" s="101" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
@@ -6837,8 +6837,8 @@
     <mergeCell ref="X3:X4"/>
     <mergeCell ref="I2:I5"/>
     <mergeCell ref="BH2:CE2"/>
+    <mergeCell ref="V3:V5"/>
     <mergeCell ref="AZ4:AZ5"/>
-    <mergeCell ref="V3:V5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="S2:S5"/>
     <mergeCell ref="AK4:AO4"/>
@@ -6900,7 +6900,7 @@
   </sheetPr>
   <dimension ref="A2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -6977,30 +6977,30 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="101" t="n"/>
+      <c r="A3" s="102" t="n"/>
       <c r="B3" s="94" t="n"/>
-      <c r="C3" s="101" t="n"/>
-      <c r="D3" s="101" t="n"/>
-      <c r="E3" s="101" t="n"/>
-      <c r="F3" s="101" t="n"/>
-      <c r="G3" s="101" t="n"/>
-      <c r="H3" s="101" t="n"/>
-      <c r="I3" s="101" t="n"/>
-      <c r="J3" s="101" t="n"/>
-      <c r="K3" s="101" t="n"/>
+      <c r="C3" s="102" t="n"/>
+      <c r="D3" s="102" t="n"/>
+      <c r="E3" s="102" t="n"/>
+      <c r="F3" s="102" t="n"/>
+      <c r="G3" s="102" t="n"/>
+      <c r="H3" s="102" t="n"/>
+      <c r="I3" s="102" t="n"/>
+      <c r="J3" s="102" t="n"/>
+      <c r="K3" s="102" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="101" t="n"/>
+      <c r="A4" s="102" t="n"/>
       <c r="B4" s="94" t="n"/>
-      <c r="C4" s="101" t="n"/>
-      <c r="D4" s="101" t="n"/>
-      <c r="E4" s="101" t="n"/>
-      <c r="F4" s="101" t="n"/>
-      <c r="G4" s="101" t="n"/>
-      <c r="H4" s="101" t="n"/>
-      <c r="I4" s="101" t="n"/>
-      <c r="J4" s="101" t="n"/>
-      <c r="K4" s="101" t="n"/>
+      <c r="C4" s="102" t="n"/>
+      <c r="D4" s="102" t="n"/>
+      <c r="E4" s="102" t="n"/>
+      <c r="F4" s="102" t="n"/>
+      <c r="G4" s="102" t="n"/>
+      <c r="H4" s="102" t="n"/>
+      <c r="I4" s="102" t="n"/>
+      <c r="J4" s="102" t="n"/>
+      <c r="K4" s="102" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="97" t="n"/>

</xml_diff>

<commit_message>
Correccion al codigo(Cesantias, incapacidades vacias, fecha liquidacion)
</commit_message>
<xml_diff>
--- a/db/excel/data.xlsx
+++ b/db/excel/data.xlsx
@@ -7030,31 +7030,31 @@
         </is>
       </c>
       <c r="D6" s="71" t="n">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="E6" s="68" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="F6" s="72">
         <f>('DATOS EMPLEADOS'!F6+'DATOS EMPLEADOS'!G6)*E6/360</f>
         <v/>
       </c>
       <c r="G6" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="H6" s="72">
         <f>('DATOS EMPLEADOS'!F6+'DATOS EMPLEADOS'!G6)*G6/360</f>
         <v/>
       </c>
       <c r="I6" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="J6" s="72">
         <f>('DATOS EMPLEADOS'!F6+'DATOS EMPLEADOS'!G6)*0.12*I6/360</f>
         <v/>
       </c>
       <c r="K6" s="66" t="n">
-        <v>45222.35011777778</v>
+        <v>45308.60041847919</v>
       </c>
     </row>
     <row r="7">
@@ -7072,31 +7072,31 @@
         </is>
       </c>
       <c r="D7" s="71" t="n">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="E7" s="68" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="F7" s="72">
         <f>('DATOS EMPLEADOS'!F7+'DATOS EMPLEADOS'!G7)*E7/360</f>
         <v/>
       </c>
       <c r="G7" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="H7" s="72">
         <f>('DATOS EMPLEADOS'!F7+'DATOS EMPLEADOS'!G7)*G7/360</f>
         <v/>
       </c>
       <c r="I7" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="J7" s="72">
         <f>('DATOS EMPLEADOS'!F7+'DATOS EMPLEADOS'!G7)*0.12*I7/360</f>
         <v/>
       </c>
       <c r="K7" s="66" t="n">
-        <v>45222.35020684028</v>
+        <v>45308.6005060795</v>
       </c>
     </row>
     <row r="8">
@@ -7156,31 +7156,31 @@
         </is>
       </c>
       <c r="D9" s="71" t="n">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="E9" s="68" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="F9" s="72">
         <f>('DATOS EMPLEADOS'!F9+'DATOS EMPLEADOS'!G9)*E9/360</f>
         <v/>
       </c>
       <c r="G9" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="H9" s="72">
         <f>('DATOS EMPLEADOS'!F9+'DATOS EMPLEADOS'!G9)*G9/360</f>
         <v/>
       </c>
       <c r="I9" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="J9" s="72">
         <f>('DATOS EMPLEADOS'!F9+'DATOS EMPLEADOS'!G9)*0.12*I9/360</f>
         <v/>
       </c>
       <c r="K9" s="66" t="n">
-        <v>45222.35027819445</v>
+        <v>45308.60057855898</v>
       </c>
     </row>
     <row r="10">
@@ -7240,31 +7240,31 @@
         </is>
       </c>
       <c r="D11" s="71" t="n">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="E11" s="68" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="F11" s="72">
         <f>('DATOS EMPLEADOS'!F11+'DATOS EMPLEADOS'!G11)*E11/360</f>
         <v/>
       </c>
       <c r="G11" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="H11" s="72">
         <f>('DATOS EMPLEADOS'!F11+'DATOS EMPLEADOS'!G11)*G11/360</f>
         <v/>
       </c>
       <c r="I11" s="68" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="J11" s="72">
         <f>('DATOS EMPLEADOS'!F11+'DATOS EMPLEADOS'!G11)*0.12*I11/360</f>
         <v/>
       </c>
       <c r="K11" s="66" t="n">
-        <v>45222.35034974537</v>
+        <v>45308.60065089612</v>
       </c>
     </row>
     <row r="12">
@@ -7282,31 +7282,31 @@
         </is>
       </c>
       <c r="D12" s="71" t="n">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="E12" s="68" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="F12" s="72">
         <f>('DATOS EMPLEADOS'!F12+'DATOS EMPLEADOS'!G12)*E12/360</f>
         <v/>
       </c>
       <c r="G12" s="68" t="n">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="H12" s="72">
         <f>('DATOS EMPLEADOS'!F12+'DATOS EMPLEADOS'!G12)*G12/360</f>
         <v/>
       </c>
       <c r="I12" s="68" t="n">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="J12" s="72">
         <f>('DATOS EMPLEADOS'!F12+'DATOS EMPLEADOS'!G12)*0.12*I12/360</f>
         <v/>
       </c>
       <c r="K12" s="66" t="n">
-        <v>45222.35042203704</v>
+        <v>45308.60072208913</v>
       </c>
     </row>
     <row r="13">

</xml_diff>